<commit_message>
FEAT: Draft pcb positions
</commit_message>
<xml_diff>
--- a/Project Outputs for KOSVT/KOSVT_BOM_Rus.xlsx
+++ b/Project Outputs for KOSVT/KOSVT_BOM_Rus.xlsx
@@ -403,7 +403,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -413,6 +413,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,14 +463,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -748,7 +755,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,7 +802,7 @@
       <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>94</v>
       </c>
       <c r="E2" s="1">
@@ -818,7 +825,7 @@
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>95</v>
       </c>
       <c r="E3" s="1">
@@ -841,7 +848,7 @@
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>96</v>
       </c>
       <c r="E4" s="1">
@@ -864,7 +871,7 @@
       <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>97</v>
       </c>
       <c r="E5" s="1">
@@ -887,7 +894,7 @@
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E6" s="1">
@@ -910,7 +917,7 @@
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
       <c r="E7" s="1">
@@ -933,7 +940,7 @@
       <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>100</v>
       </c>
       <c r="E8" s="1">
@@ -956,7 +963,7 @@
       <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>101</v>
       </c>
       <c r="E9" s="1">
@@ -998,7 +1005,7 @@
       <c r="C11" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="7" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="1">
@@ -1040,7 +1047,7 @@
       <c r="C13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>102</v>
       </c>
       <c r="E13" s="1">
@@ -1061,7 +1068,7 @@
       <c r="C14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>103</v>
       </c>
       <c r="E14" s="1">
@@ -1082,7 +1089,7 @@
       <c r="C15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>104</v>
       </c>
       <c r="E15" s="1">
@@ -1128,7 +1135,7 @@
       <c r="C17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>105</v>
       </c>
       <c r="E17" s="1">
@@ -1151,7 +1158,7 @@
       <c r="C18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>106</v>
       </c>
       <c r="E18" s="1">
@@ -1174,7 +1181,7 @@
       <c r="C19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E19" s="1">
@@ -1197,7 +1204,7 @@
       <c r="C20" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="6" t="s">
         <v>108</v>
       </c>
       <c r="E20" s="1">
@@ -1220,7 +1227,7 @@
       <c r="C21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>109</v>
       </c>
       <c r="E21" s="1">
@@ -1243,7 +1250,7 @@
       <c r="C22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E22" s="1">
@@ -1266,7 +1273,7 @@
       <c r="C23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>111</v>
       </c>
       <c r="E23" s="1">
@@ -1329,7 +1336,7 @@
       <c r="C26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="6" t="s">
         <v>112</v>
       </c>
       <c r="E26" s="1">
@@ -1478,7 +1485,7 @@
       <c r="C33" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E33" s="1">
@@ -1487,7 +1494,7 @@
       <c r="F33" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="6" t="s">
+      <c r="G33" s="5" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>